<commit_message>
Updated the mapping file (CatVarDict.xlsx)
</commit_message>
<xml_diff>
--- a/scripts/summarize/inputs/calibration/CatVarDict.xlsx
+++ b/scripts/summarize/inputs/calibration/CatVarDict.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BKRCast_Support\ModeChoice\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A01263F-BE80-4A65-A56B-23F8A60C71E4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="585" windowWidth="18195" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="1410" yWindow="585" windowWidth="18195" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Household" sheetId="1" r:id="rId1"/>
@@ -377,7 +383,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,6 +426,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -468,7 +477,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,9 +510,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -536,6 +562,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -711,7 +754,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -849,7 +892,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1204,7 +1247,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1283,11 +1326,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,7 +1562,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="I8">
         <v>6</v>
@@ -1569,6 +1612,7 @@
       <c r="B11" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1584,7 +1628,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">

</xml_diff>

<commit_message>
code for 2018 bkrcast calibrated model
</commit_message>
<xml_diff>
--- a/scripts/summarize/inputs/calibration/CatVarDict.xlsx
+++ b/scripts/summarize/inputs/calibration/CatVarDict.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BKRCast_Support\ModeChoice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BKRCast2014R1-test11a1\scripts\summarize\inputs\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A01263F-BE80-4A65-A56B-23F8A60C71E4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="585" windowWidth="18195" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="585" windowWidth="18195" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Household" sheetId="1" r:id="rId1"/>
@@ -383,7 +382,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -754,7 +753,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -892,7 +891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1247,7 +1246,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1326,7 +1325,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1628,7 +1627,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">

</xml_diff>

<commit_message>
Added fixes to the tnc mode implementation. Main fix is in the balancing trips.
</commit_message>
<xml_diff>
--- a/scripts/summarize/inputs/calibration/CatVarDict.xlsx
+++ b/scripts/summarize/inputs/calibration/CatVarDict.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BKRCast2014R1-test11a1\scripts\summarize\inputs\calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Clients\BKR\GitRunModel\scripts\summarize\inputs\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="585" windowWidth="18195" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="1410" yWindow="585" windowWidth="18195" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Household" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="122">
   <si>
     <t>hownrent</t>
   </si>
@@ -377,6 +377,18 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Driver+Passenger</t>
+  </si>
+  <si>
+    <t>Driver+2Passengers</t>
+  </si>
+  <si>
+    <t>Driver+3+Passengers</t>
+  </si>
+  <si>
+    <t>PRS</t>
   </si>
 </sst>
 </file>
@@ -420,8 +432,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -509,23 +549,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -561,23 +584,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1328,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,6 +1887,12 @@
       <c r="L6" s="2" t="s">
         <v>111</v>
       </c>
+      <c r="M6">
+        <v>11</v>
+      </c>
+      <c r="N6" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1919,6 +1931,12 @@
       <c r="L7" s="2" t="s">
         <v>112</v>
       </c>
+      <c r="M7">
+        <v>12</v>
+      </c>
+      <c r="N7" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1944,6 +1962,12 @@
       </c>
       <c r="L8" s="2" t="s">
         <v>113</v>
+      </c>
+      <c r="M8">
+        <v>13</v>
+      </c>
+      <c r="N8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1963,7 +1987,7 @@
         <v>9</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>6</v>
+        <v>121</v>
       </c>
       <c r="K9">
         <v>7</v>

</xml_diff>